<commit_message>
add results of same initialization version of v1
</commit_message>
<xml_diff>
--- a/v1+/mse/regression.xlsx
+++ b/v1+/mse/regression.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Desktop\master\ensemble_github\experimental_data\v1+\mse\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{621BFC3B-B4B0-4778-8653-F066EE82AAD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23675846-56FA-4915-9585-565805441202}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2280" yWindow="1510" windowWidth="23970" windowHeight="19490" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1453,11 +1453,11 @@
     <t>-4.03%</t>
   </si>
   <si>
-    <t>v1+(same initialization):standard version</t>
+    <t>v1:standard version</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
-    <t>v1:standard version</t>
+    <t>v1+(same initialization):mse in phase 1</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
 </sst>
@@ -1902,7 +1902,7 @@
   <dimension ref="A1:I92"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="C1" sqref="C1:E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.25"/>
@@ -1918,12 +1918,12 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C1" s="12" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="D1" s="12"/>
       <c r="E1" s="12"/>
       <c r="G1" s="12" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="H1" s="12"/>
       <c r="I1" s="12"/>

</xml_diff>